<commit_message>
creating a false BU to check user permissions to delete
</commit_message>
<xml_diff>
--- a/dbs/database.eamena/data/bulk_data/bu_files/my_false_bu.xlsx
+++ b/dbs/database.eamena/data/bulk_data/bu_files/my_false_bu.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas Huet\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rprojects\eamena-arches-dev\dbs\database.eamena\data\bulk_data\bu_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F481B6C-F339-49FE-A604-F64D56C94B50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F124572-44E6-4087-B1CE-27AFE7680485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" tabRatio="862" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -508,16 +508,16 @@
     <t>MyTestHP</t>
   </si>
   <si>
-    <t>Alternative Name</t>
-  </si>
-  <si>
     <t>POINT(20 36)</t>
   </si>
   <si>
     <t>Thomas Huet</t>
   </si>
   <si>
-    <t>ThisGridIdIsFalse-00</t>
+    <t>Alternative Reference</t>
+  </si>
+  <si>
+    <t>E30N29-12</t>
   </si>
 </sst>
 </file>
@@ -527,7 +527,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -599,6 +599,12 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -873,7 +879,7 @@
     <xf numFmtId="0" fontId="5" fillId="13" borderId="1" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="4" applyFont="1" applyAlignment="1">
@@ -971,80 +977,81 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="16" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="1" xfId="6" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="7" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="1" xfId="8" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="9" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="10" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="11" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="15" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="12" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="1" xfId="13" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="14" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="10" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="1" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="1" xfId="13" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="1" xfId="11" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="1" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="10" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="1" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="1" xfId="13" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="1" xfId="11" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="7" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="1" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="16" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="1" xfId="6" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="1" xfId="8" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="9" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="10" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="11" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="15" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="12" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="1" xfId="13" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="14" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="18">
     <cellStyle name="20% - Accent2 2" xfId="5" xr:uid="{A1F8C98C-AF1C-464F-8ABE-8343A54B283F}"/>
@@ -1287,10 +1294,10 @@
   <dimension ref="A1:CU7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomRight" activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.7265625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1361,117 +1368,117 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:99" x14ac:dyDescent="0.3">
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="47" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="51" t="s">
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="62" t="s">
         <v>77</v>
       </c>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="51"/>
-      <c r="P1" s="51"/>
-      <c r="Q1" s="51"/>
-      <c r="R1" s="51"/>
-      <c r="S1" s="51"/>
-      <c r="T1" s="52" t="s">
+      <c r="K1" s="62"/>
+      <c r="L1" s="62"/>
+      <c r="M1" s="62"/>
+      <c r="N1" s="62"/>
+      <c r="O1" s="62"/>
+      <c r="P1" s="62"/>
+      <c r="Q1" s="62"/>
+      <c r="R1" s="62"/>
+      <c r="S1" s="62"/>
+      <c r="T1" s="63" t="s">
         <v>78</v>
       </c>
-      <c r="U1" s="52"/>
-      <c r="V1" s="52"/>
-      <c r="W1" s="52"/>
-      <c r="X1" s="53" t="s">
+      <c r="U1" s="63"/>
+      <c r="V1" s="63"/>
+      <c r="W1" s="63"/>
+      <c r="X1" s="64" t="s">
         <v>79</v>
       </c>
-      <c r="Y1" s="53"/>
-      <c r="Z1" s="53"/>
-      <c r="AA1" s="53"/>
-      <c r="AB1" s="53"/>
-      <c r="AC1" s="53"/>
-      <c r="AD1" s="53"/>
-      <c r="AE1" s="53"/>
-      <c r="AF1" s="53"/>
-      <c r="AG1" s="58" t="s">
+      <c r="Y1" s="64"/>
+      <c r="Z1" s="64"/>
+      <c r="AA1" s="64"/>
+      <c r="AB1" s="64"/>
+      <c r="AC1" s="64"/>
+      <c r="AD1" s="64"/>
+      <c r="AE1" s="64"/>
+      <c r="AF1" s="64"/>
+      <c r="AG1" s="45" t="s">
         <v>80</v>
       </c>
-      <c r="AH1" s="58"/>
-      <c r="AI1" s="58"/>
-      <c r="AJ1" s="58"/>
-      <c r="AK1" s="58"/>
-      <c r="AL1" s="58"/>
-      <c r="AM1" s="58"/>
-      <c r="AN1" s="58"/>
-      <c r="AO1" s="58"/>
-      <c r="AP1" s="58"/>
-      <c r="AQ1" s="58"/>
-      <c r="AR1" s="58"/>
-      <c r="AS1" s="58"/>
-      <c r="AT1" s="58"/>
-      <c r="AU1" s="58"/>
-      <c r="AV1" s="58"/>
-      <c r="AW1" s="58"/>
-      <c r="AX1" s="58"/>
-      <c r="AY1" s="58"/>
-      <c r="AZ1" s="58"/>
-      <c r="BA1" s="58"/>
-      <c r="BB1" s="58"/>
-      <c r="BC1" s="58"/>
-      <c r="BD1" s="58"/>
-      <c r="BE1" s="58"/>
-      <c r="BF1" s="58"/>
-      <c r="BG1" s="58"/>
-      <c r="BH1" s="58"/>
-      <c r="BI1" s="58"/>
-      <c r="BJ1" s="58"/>
-      <c r="BK1" s="58"/>
-      <c r="BL1" s="58"/>
-      <c r="BM1" s="58"/>
-      <c r="BN1" s="66" t="s">
+      <c r="AH1" s="45"/>
+      <c r="AI1" s="45"/>
+      <c r="AJ1" s="45"/>
+      <c r="AK1" s="45"/>
+      <c r="AL1" s="45"/>
+      <c r="AM1" s="45"/>
+      <c r="AN1" s="45"/>
+      <c r="AO1" s="45"/>
+      <c r="AP1" s="45"/>
+      <c r="AQ1" s="45"/>
+      <c r="AR1" s="45"/>
+      <c r="AS1" s="45"/>
+      <c r="AT1" s="45"/>
+      <c r="AU1" s="45"/>
+      <c r="AV1" s="45"/>
+      <c r="AW1" s="45"/>
+      <c r="AX1" s="45"/>
+      <c r="AY1" s="45"/>
+      <c r="AZ1" s="45"/>
+      <c r="BA1" s="45"/>
+      <c r="BB1" s="45"/>
+      <c r="BC1" s="45"/>
+      <c r="BD1" s="45"/>
+      <c r="BE1" s="45"/>
+      <c r="BF1" s="45"/>
+      <c r="BG1" s="45"/>
+      <c r="BH1" s="45"/>
+      <c r="BI1" s="45"/>
+      <c r="BJ1" s="45"/>
+      <c r="BK1" s="45"/>
+      <c r="BL1" s="45"/>
+      <c r="BM1" s="45"/>
+      <c r="BN1" s="54" t="s">
         <v>81</v>
       </c>
-      <c r="BO1" s="66"/>
-      <c r="BP1" s="66"/>
-      <c r="BQ1" s="66"/>
-      <c r="BR1" s="66"/>
-      <c r="BS1" s="66"/>
-      <c r="BT1" s="66"/>
-      <c r="BU1" s="66"/>
-      <c r="BV1" s="66"/>
-      <c r="BW1" s="66"/>
-      <c r="BX1" s="66"/>
-      <c r="BY1" s="66"/>
-      <c r="BZ1" s="66"/>
-      <c r="CA1" s="66"/>
-      <c r="CB1" s="66"/>
-      <c r="CC1" s="66"/>
-      <c r="CD1" s="66"/>
-      <c r="CE1" s="66"/>
-      <c r="CF1" s="66"/>
-      <c r="CG1" s="66"/>
-      <c r="CH1" s="44" t="s">
+      <c r="BO1" s="54"/>
+      <c r="BP1" s="54"/>
+      <c r="BQ1" s="54"/>
+      <c r="BR1" s="54"/>
+      <c r="BS1" s="54"/>
+      <c r="BT1" s="54"/>
+      <c r="BU1" s="54"/>
+      <c r="BV1" s="54"/>
+      <c r="BW1" s="54"/>
+      <c r="BX1" s="54"/>
+      <c r="BY1" s="54"/>
+      <c r="BZ1" s="54"/>
+      <c r="CA1" s="54"/>
+      <c r="CB1" s="54"/>
+      <c r="CC1" s="54"/>
+      <c r="CD1" s="54"/>
+      <c r="CE1" s="54"/>
+      <c r="CF1" s="54"/>
+      <c r="CG1" s="54"/>
+      <c r="CH1" s="56" t="s">
         <v>82</v>
       </c>
-      <c r="CI1" s="44"/>
-      <c r="CJ1" s="44"/>
-      <c r="CK1" s="44"/>
-      <c r="CL1" s="44"/>
-      <c r="CM1" s="44"/>
-      <c r="CN1" s="44"/>
-      <c r="CO1" s="44"/>
-      <c r="CP1" s="44"/>
-      <c r="CQ1" s="44"/>
-      <c r="CR1" s="44"/>
-      <c r="CS1" s="44"/>
-      <c r="CT1" s="44"/>
+      <c r="CI1" s="56"/>
+      <c r="CJ1" s="56"/>
+      <c r="CK1" s="56"/>
+      <c r="CL1" s="56"/>
+      <c r="CM1" s="56"/>
+      <c r="CN1" s="56"/>
+      <c r="CO1" s="56"/>
+      <c r="CP1" s="56"/>
+      <c r="CQ1" s="56"/>
+      <c r="CR1" s="56"/>
+      <c r="CS1" s="56"/>
+      <c r="CT1" s="56"/>
       <c r="CU1" s="2" t="s">
         <v>83</v>
       </c>
@@ -1479,32 +1486,32 @@
     <row r="2" spans="1:99" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
-      <c r="D2" s="59" t="s">
+      <c r="D2" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="45" t="s">
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="57" t="s">
         <v>85</v>
       </c>
-      <c r="K2" s="45"/>
+      <c r="K2" s="57"/>
       <c r="L2" s="4"/>
-      <c r="M2" s="46" t="s">
+      <c r="M2" s="52" t="s">
         <v>86</v>
       </c>
-      <c r="N2" s="46"/>
-      <c r="O2" s="47" t="s">
+      <c r="N2" s="52"/>
+      <c r="O2" s="58" t="s">
         <v>87</v>
       </c>
-      <c r="P2" s="47"/>
-      <c r="Q2" s="48" t="s">
+      <c r="P2" s="58"/>
+      <c r="Q2" s="59" t="s">
         <v>88</v>
       </c>
-      <c r="R2" s="48"/>
-      <c r="S2" s="48"/>
+      <c r="R2" s="59"/>
+      <c r="S2" s="59"/>
       <c r="T2" s="5"/>
       <c r="U2" s="5"/>
       <c r="V2" s="5"/>
@@ -1514,104 +1521,104 @@
       <c r="Z2" s="7"/>
       <c r="AA2" s="6"/>
       <c r="AB2" s="6"/>
-      <c r="AC2" s="48" t="s">
+      <c r="AC2" s="59" t="s">
         <v>89</v>
       </c>
-      <c r="AD2" s="48"/>
-      <c r="AE2" s="49" t="s">
+      <c r="AD2" s="59"/>
+      <c r="AE2" s="60" t="s">
         <v>90</v>
       </c>
-      <c r="AF2" s="49"/>
+      <c r="AF2" s="60"/>
       <c r="AG2" s="8"/>
       <c r="AH2" s="8"/>
-      <c r="AI2" s="50" t="s">
+      <c r="AI2" s="61" t="s">
         <v>91</v>
       </c>
-      <c r="AJ2" s="50"/>
-      <c r="AK2" s="50"/>
-      <c r="AL2" s="50"/>
+      <c r="AJ2" s="61"/>
+      <c r="AK2" s="61"/>
+      <c r="AL2" s="61"/>
       <c r="AM2" s="19"/>
-      <c r="AN2" s="64" t="s">
+      <c r="AN2" s="51" t="s">
         <v>139</v>
       </c>
-      <c r="AO2" s="64"/>
-      <c r="AP2" s="64"/>
-      <c r="AQ2" s="64"/>
-      <c r="AR2" s="64"/>
-      <c r="AS2" s="64"/>
-      <c r="AT2" s="64"/>
-      <c r="AU2" s="64"/>
-      <c r="AV2" s="46" t="s">
+      <c r="AO2" s="51"/>
+      <c r="AP2" s="51"/>
+      <c r="AQ2" s="51"/>
+      <c r="AR2" s="51"/>
+      <c r="AS2" s="51"/>
+      <c r="AT2" s="51"/>
+      <c r="AU2" s="51"/>
+      <c r="AV2" s="52" t="s">
         <v>92</v>
       </c>
-      <c r="AW2" s="46"/>
-      <c r="AX2" s="46"/>
-      <c r="AY2" s="46"/>
-      <c r="AZ2" s="46"/>
-      <c r="BA2" s="46"/>
-      <c r="BB2" s="46"/>
-      <c r="BC2" s="46"/>
-      <c r="BD2" s="46"/>
-      <c r="BE2" s="46"/>
-      <c r="BF2" s="65" t="s">
+      <c r="AW2" s="52"/>
+      <c r="AX2" s="52"/>
+      <c r="AY2" s="52"/>
+      <c r="AZ2" s="52"/>
+      <c r="BA2" s="52"/>
+      <c r="BB2" s="52"/>
+      <c r="BC2" s="52"/>
+      <c r="BD2" s="52"/>
+      <c r="BE2" s="52"/>
+      <c r="BF2" s="53" t="s">
         <v>145</v>
       </c>
-      <c r="BG2" s="65"/>
-      <c r="BH2" s="65"/>
-      <c r="BI2" s="62" t="s">
+      <c r="BG2" s="53"/>
+      <c r="BH2" s="53"/>
+      <c r="BI2" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="BJ2" s="62"/>
-      <c r="BK2" s="62"/>
-      <c r="BL2" s="62"/>
+      <c r="BJ2" s="49"/>
+      <c r="BK2" s="49"/>
+      <c r="BL2" s="49"/>
       <c r="BM2" s="8"/>
       <c r="BN2" s="9"/>
       <c r="BO2" s="9"/>
-      <c r="BP2" s="55" t="s">
+      <c r="BP2" s="66" t="s">
         <v>93</v>
       </c>
-      <c r="BQ2" s="55"/>
-      <c r="BR2" s="55"/>
-      <c r="BS2" s="55"/>
-      <c r="BT2" s="55"/>
-      <c r="BU2" s="55"/>
-      <c r="BV2" s="55"/>
-      <c r="BW2" s="55"/>
-      <c r="BX2" s="55"/>
-      <c r="BY2" s="55"/>
-      <c r="BZ2" s="56" t="s">
+      <c r="BQ2" s="66"/>
+      <c r="BR2" s="66"/>
+      <c r="BS2" s="66"/>
+      <c r="BT2" s="66"/>
+      <c r="BU2" s="66"/>
+      <c r="BV2" s="66"/>
+      <c r="BW2" s="66"/>
+      <c r="BX2" s="66"/>
+      <c r="BY2" s="66"/>
+      <c r="BZ2" s="67" t="s">
         <v>94</v>
       </c>
-      <c r="CA2" s="56"/>
-      <c r="CB2" s="56"/>
+      <c r="CA2" s="67"/>
+      <c r="CB2" s="67"/>
       <c r="CC2" s="18"/>
-      <c r="CD2" s="63" t="s">
+      <c r="CD2" s="50" t="s">
         <v>148</v>
       </c>
-      <c r="CE2" s="63"/>
-      <c r="CF2" s="63"/>
+      <c r="CE2" s="50"/>
+      <c r="CF2" s="50"/>
       <c r="CG2" s="20"/>
       <c r="CH2" s="10"/>
-      <c r="CI2" s="57" t="s">
+      <c r="CI2" s="68" t="s">
         <v>95</v>
       </c>
-      <c r="CJ2" s="57"/>
-      <c r="CK2" s="61" t="s">
+      <c r="CJ2" s="68"/>
+      <c r="CK2" s="48" t="s">
         <v>96</v>
       </c>
-      <c r="CL2" s="61"/>
+      <c r="CL2" s="48"/>
       <c r="CM2" s="10"/>
-      <c r="CN2" s="54" t="s">
+      <c r="CN2" s="65" t="s">
         <v>97</v>
       </c>
-      <c r="CO2" s="54"/>
-      <c r="CP2" s="54"/>
-      <c r="CQ2" s="43" t="s">
+      <c r="CO2" s="65"/>
+      <c r="CP2" s="65"/>
+      <c r="CQ2" s="55" t="s">
         <v>98</v>
       </c>
-      <c r="CR2" s="43"/>
-      <c r="CS2" s="43"/>
-      <c r="CT2" s="43"/>
+      <c r="CR2" s="55"/>
+      <c r="CS2" s="55"/>
+      <c r="CT2" s="55"/>
       <c r="CU2" s="11"/>
     </row>
     <row r="3" spans="1:99" s="12" customFormat="1" ht="34.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1918,7 +1925,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="42" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C4" s="42" t="s">
         <v>1</v>
@@ -1937,11 +1944,11 @@
       </c>
       <c r="H4" s="15"/>
       <c r="I4" s="15"/>
-      <c r="J4" t="s">
+      <c r="J4" s="69" t="s">
         <v>160</v>
       </c>
-      <c r="K4" s="67" t="s">
-        <v>161</v>
+      <c r="K4" s="43" t="s">
+        <v>163</v>
       </c>
       <c r="L4" t="s">
         <v>6</v>
@@ -1962,7 +1969,7 @@
       <c r="R4"/>
       <c r="S4"/>
       <c r="T4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="U4" t="s">
         <v>20</v>
@@ -2203,20 +2210,10 @@
       <c r="CJ5" s="21"/>
     </row>
     <row r="7" spans="1:99" x14ac:dyDescent="0.3">
-      <c r="G7" s="68"/>
+      <c r="G7" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="AG1:BM1"/>
-    <mergeCell ref="D2:I2"/>
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="CK2:CL2"/>
-    <mergeCell ref="BI2:BL2"/>
-    <mergeCell ref="CD2:CF2"/>
-    <mergeCell ref="AN2:AU2"/>
-    <mergeCell ref="AV2:BE2"/>
-    <mergeCell ref="BF2:BH2"/>
-    <mergeCell ref="BN1:CG1"/>
     <mergeCell ref="CQ2:CT2"/>
     <mergeCell ref="CH1:CT1"/>
     <mergeCell ref="J2:K2"/>
@@ -2233,433 +2230,26 @@
     <mergeCell ref="BP2:BY2"/>
     <mergeCell ref="BZ2:CB2"/>
     <mergeCell ref="CI2:CJ2"/>
+    <mergeCell ref="AG1:BM1"/>
+    <mergeCell ref="D2:I2"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="CK2:CL2"/>
+    <mergeCell ref="BI2:BL2"/>
+    <mergeCell ref="CD2:CF2"/>
+    <mergeCell ref="AN2:AU2"/>
+    <mergeCell ref="AV2:BE2"/>
+    <mergeCell ref="BF2:BH2"/>
+    <mergeCell ref="BN1:CG1"/>
   </mergeCells>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI4:AI5" xr:uid="{EED91AFD-5A27-4095-AD7C-75DEAD76AB85}">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K5:K117 Z4:Z1048576 AD4:AD94 AG4:AH117 BJ4:BL111 BF4:BH53 BN4:BO117 AV4:AW1048576 CH4:CI117 CK4:CP117 O4:P117 L4:M1048576 AF5:AF74 C5:C137 D5:D117 BZ6:BZ117 BP4:BP150 BQ4:BQ131 BC1:BC1048576 AX1:AY1048576 BA4:BA5 Q4:Q5 CD4:CF1048576 CA6:CB1048576 BX6:BY1048576 BA6:BB1048576 AI6:AI1048576 AB4:AB1048576 U4:X1048576 F6:F1048576 AK6:AL1048576 AJ4:AJ131 CS4:CS117 BS116:BS117 BU116:BV117 BR4:BR117" xr:uid="{6A7EB0D8-16D6-4BC1-9AA7-3F55327D4A59}">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="69">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6A7EB0D8-16D6-4BC1-9AA7-3F55327D4A59}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>CI107:CI117</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{48A5322C-F214-4A49-A037-884666AE59D2}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>CM21:CM117</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F738DB1E-57D9-46A8-B85D-C3F8A7F2C48D}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>CN53:CN117</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B7FEBD52-32AF-4013-AD0F-BCE6AA501BB2}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>CO53:CP117</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{91A8F9CA-2FF4-4E84-A240-1F193A6269AD}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>BS116:BS117 BU116:BV117 BR4:BR117</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7A4B8751-605B-4A9F-9194-5F3D1CADBB80}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>CH6:CH117</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7BC642EB-CB2E-4C1B-9600-A1C84FB323C4}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>CK6:CK117</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2806FC1F-7A35-4DF7-B926-305C302A16A1}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>CL6:CL117</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EADD464A-E111-4085-898A-690F1F369013}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>CS6:CS117</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F0D12797-2899-4738-BE63-E945055399A5}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>AL6:AL1048576 AJ4:AJ131</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BC9B4932-70C3-4A41-9E65-CB40C82C2146}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>F6:F1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3C78738E-D068-40D7-9D50-EF0FAB6BB07D}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>U6:U1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4C4064FB-61C8-4CDE-904E-23E121E5C0AC}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>X6:X1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DE7665E7-E247-4AE6-83BA-F293424DB996}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>AB6:AB1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3F374C89-1E13-4916-96F8-CCBD26DBCC7A}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>AK6:AK1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{62D66CA2-A767-4351-9DB7-ACEB9A4BE7D3}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>AI6:AI1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6D45406E-B848-40DD-B0A2-05EA79CA1142}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>BA6:BA1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7D6B8343-91A8-4183-9DA4-36368838E36D}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>BB6:BB1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2E82F648-CE4A-4EB3-9B65-8A0A161BE0E2}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>BX6:BX1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4AD7188E-5E45-4B80-8642-2B84E4E29DEA}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>BY6:BY1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0AFF0338-ADDE-494A-AB4C-205BC21A09D9}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>CB6:CB1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BD33F52C-7BEB-42A2-82FF-6427B6E1E857}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>CD6:CD1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5BF09B6B-565F-47CA-90D5-D37DA1C6BFC3}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>CE6:CE1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D75F373A-1F2B-4E68-A95C-D91F81A015CA}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>CF6:CF1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8409593E-673D-465F-997C-F0334FFBD090}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>CH4:CH5</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A6B01578-DB0D-4270-A9DE-5B93A93926AB}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>CD4:CD5</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{58B3CCEC-CBAC-46AA-9CAE-F1ECB4E93EFE}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>CE4:CE5</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CFB4E3E7-1B1D-46AC-9D42-51CDB467097D}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>CF4:CF5</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{83966C89-F404-4ADB-B4EA-55EC51BEDDB5}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>CK4:CK5</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{073476B6-04D4-4BA8-9610-B018F44BEDDB}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>CL4:CL5</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3D0E9659-99C1-44DF-94B7-E51157F92DCD}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>Q4:Q5</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FE7E74CA-4FCB-4A00-9DF4-B45D7B20A066}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>U4:U5</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{11525CC8-C3CA-475E-B5F8-2684024AB49B}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>X4:X5</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F6354FC6-53B8-4FC4-B276-BA28BC3E1E30}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>AB4:AB5</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{313CD640-5F6F-4A60-B226-2DCC8F8606AE}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>CS4:CS5</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1D6E6110-4928-49F5-9E7C-A045F7F3C50A}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>BA4:BA5</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3198E08C-C329-4454-B683-23F360A1BF94}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>AX1:AX1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{16B79779-2029-40B3-AB50-F427CB0FA22F}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>AY1:AY1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EFE233DE-9637-6249-AC9D-686CE335105F}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>BC1:BC1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AE95CF08-6270-4892-83F5-1B623954BBA3}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>BQ4:BQ131 CA6:CA1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D3305EAF-CEFD-4981-BDC2-1F640AAB0AD8}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>BZ6:BZ117 BP4:BP150</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8BD47373-1382-4A7D-8864-ABBD21BB21A4}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>D5:D117</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9866C7DB-DFAA-4CFD-AAC2-36CDB1EF3D2C}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>C5:C137</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D42690B5-57FD-4FA0-BC60-EC6EBBD22B15}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>AF5:AF74</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E0348F7C-F057-45A4-A882-1A477AB8EDAB}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>L4:L1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{485E8B1E-C243-4335-B711-ED8C0A2A3B10}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>O4:O117</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{553E4C36-06F6-49CF-81BF-84ED26A7D6DF}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>P4:P117</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FF74694F-AA44-4E04-8BB6-F6AAD62E6B20}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>CP4:CP52</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DFC94441-6F27-4F41-8B21-156C52B9ED7F}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>CI4:CI106</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BA0BD8EB-05E4-4710-83DD-AF8363A8F76E}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>CM4:CM20</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D3E795B3-CD70-443E-BA94-A3FD9EEC32AE}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>CN4:CN52</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D3DEBD25-B74B-4D34-A1B7-C7417B26F88C}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>CO4:CO52</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{07445BB1-0B67-4235-A5F4-385B24B7DDC6}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>AW4:AW1048576 M4:M1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E5F05B73-6D7E-47B4-8B8A-90CF0F46D071}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>BN4:BN117</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DC2F5362-4B0F-4828-A1F0-387BA66D9003}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>BO4:BO117</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AF271434-689D-4740-82A0-C73B042A9DC8}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>BF4:BF53</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{21892EFF-0D97-44E2-93D6-896E5C9A626D}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>BG4:BG53</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{79438F74-0BF6-4879-8DF4-C40E780A7254}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>BH4:BH53</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AB850895-FAD9-4300-8DAB-D31349771104}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>BJ4:BJ111</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3F8990BD-79FC-4E62-8994-2568BB164BB3}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>BK4:BK111</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{41C68B62-E6F7-4126-867F-52FA46C18973}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>BL4:BL111</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C3B4B94F-CE9B-4E78-95C5-69A3198F280C}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>AG4:AG117</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{361D3192-4604-47FB-8680-352371E97CE6}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>AH4:AH117</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{11484FB7-4809-4C47-A299-42482ECC8724}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>AD4:AD94</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{ADDC1195-43BD-4AD5-9994-00B3936CEC76}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>W4:W1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5A7DA80E-F586-4F63-9D19-0D261DFD97C8}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>V4:V1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9A97B0A5-B3B8-4FBD-A6E3-E6BA5D675500}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>Z4:Z1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F8992A07-E289-4C25-9116-B6498629391C}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>AV4:AV1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DC06C25E-167F-47A3-891A-EF07A0133A20}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>K5:K117</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>